<commit_message>
Agrega evidencia Fase 3 y actualiza documentacion
</commit_message>
<xml_diff>
--- a/Fase 2/Evidencias Grupales/PLANILLA DE EVALUACION AVANCE FASE 2.xlsx
+++ b/Fase 2/Evidencias Grupales/PLANILLA DE EVALUACION AVANCE FASE 2.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arturoguerra/Library/Mobile Documents/com~apple~CloudDocs/Capstone Seccionn 7/Fase 2 Avance/Grupo 1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arturoguerra/Library/Mobile Documents/com~apple~CloudDocs/Capstone Seccionn 7/Fase 2 Final/Grupo 1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B50D98B-CE56-6746-BBDB-667353FADFB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{350672B5-20C3-FF47-A0AF-034F064C0922}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2300" yWindow="3160" windowWidth="32260" windowHeight="17280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="31780" windowHeight="20360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="EVALUACION2" sheetId="1" r:id="rId1"/>
-    <sheet name="RUBRICA" sheetId="12" r:id="rId2"/>
+    <sheet name="RUBRICA" sheetId="12" r:id="rId1"/>
+    <sheet name="EVALUACION1" sheetId="1" r:id="rId2"/>
     <sheet name="ESCALA_IEP" sheetId="2" state="hidden" r:id="rId3"/>
     <sheet name="ESCALA_PRESENTACION" sheetId="3" state="hidden" r:id="rId4"/>
     <sheet name="ESCALA_TRAB_EQUIP" sheetId="4" state="hidden" r:id="rId5"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="91">
   <si>
     <t>PUNTOS</t>
   </si>
@@ -105,6 +105,18 @@
   </si>
   <si>
     <t>Nota</t>
+  </si>
+  <si>
+    <t>PUNTAJE</t>
+  </si>
+  <si>
+    <t>INDIVIDUAL</t>
+  </si>
+  <si>
+    <t>NOMBRE ALUMNO</t>
+  </si>
+  <si>
+    <t>Capacidad de Trabajo en Equipo</t>
   </si>
   <si>
     <t>Indicador de Evaluación</t>
@@ -167,73 +179,94 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">1. Propone ajustes al Proyecto APT considerando dificultades, facilitadores y retroalimentación. </t>
+    <t>1. Implementa una metodología que permite el logro de los objetivos propuestos, de acuerdo a los estándares de la disciplina.</t>
   </si>
   <si>
-    <t>Señala los ajustes que realizó o realizará y los justifica considerando las dificultades, facilitadores y retroalimentación del docente.</t>
+    <t xml:space="preserve">Describe la metodología utilizada de acuerdo a los estándares de la disciplina, alcanzando todos los objetivos propuestos para el proyecto. </t>
   </si>
   <si>
-    <t>Señala algunos de los ajustes que realizó o realizará y los justifica considerando las dificultades, facilitadores o retroalimentación del docente.</t>
+    <t xml:space="preserve">Describe la metodología utilizada de acuerdo a los estándares de la disciplina, pero cumple parcialmente los objetivos propuestos para el proyecto. </t>
   </si>
   <si>
-    <t>Señala los ajustes que realizó o realizará, pero no los justifica.</t>
+    <t xml:space="preserve">Describe la metodología utilizada cumpliendo parcialmente con los estándares de la disciplina y con los objetivos propuestos para el proyecto. </t>
   </si>
   <si>
-    <t>No incluye ajustes ni justifica por qué mantiene su plan inicial.</t>
+    <t xml:space="preserve">Describe la metodología utilizada sin cumplir los estándares de la disciplina ni los objetivos propuestos para el proyecto. </t>
   </si>
   <si>
-    <t>2. Aplica una metodología que permite el logro de los objetivos propuestos, de acuerdo a los estándares de la disciplina.</t>
+    <t xml:space="preserve">6. Utiliza correctamente las reglas de redacción, ortografía (literal, puntual, acentual) y las normas para citas y referencias. </t>
   </si>
   <si>
-    <t xml:space="preserve">Aplica la metodología definida de acuerdo a los estándares de la disciplina, pero no se observa el cumplimiento de objetivos propuestos para el avance del proyecto. </t>
+    <t>Expone el tema utilizando un lenguaje técnico disciplinar al presentar la propuesta y responde evidenciando un manejo de la información la mayoría del tiempo.</t>
   </si>
   <si>
-    <t xml:space="preserve">Aplica la metodología definida cumpliendo parcialmente con los estándares de la disciplina y con los objetivos propuestos para el avance del proyecto. </t>
+    <t>Expone el tema utilizando un lenguaje técnico disciplinar al presentar la propuesta y responde evidenciando un manejo de la información la mitad del tiempo.</t>
   </si>
   <si>
-    <t xml:space="preserve">Aplica la metodología definida sin cumplir los estándares de la disciplina ni los objetivos propuestos para el avance del proyecto. </t>
+    <t>Expone el tema utilizando un lenguaje técnico disciplinar al presentar la propuesta y responde evidenciando un manejo de la información en menos de la mitad del tiempo.</t>
   </si>
   <si>
-    <t xml:space="preserve">5. Utiliza reglas de redacción, ortografía (literal, puntual, acentual) y las normas para citas y referencias. </t>
+    <t>El estudiante realiza un excelente trabajo en equipo, fomentando un ambiente positivo, siendo participativo con su equipo en las sesiones presenciales de la asignatura y participando de manera equitativa en la presentación del caso</t>
   </si>
   <si>
-    <t>8. Demuestra un trabajo en equipo en donde todos los miembros del equipo expresan con fluidez el conocimiento del tema expuesto y  participan de las actividades planificadas en el proyecto</t>
+    <t xml:space="preserve">El estudiante realiza un buen trabajo en equipo, fomentando un ambiente positivo, siendo participativo con su equipo en las sesiones presenciales de la asignatura, pero no demuestra una participación de manera equitativa en la presentación del caso </t>
   </si>
   <si>
-    <t>Demuestra un trabajo en equipo en donde todos los miembros del equipo expresan con fluidez el conocimiento del tema expuesto y  participan de las actividades planificadas en el proyecto</t>
+    <t>El estudiante realiza un trabajo deficiente con el equipo, fomentando un ambiente positivo pero no demuestra ser participativo con su equipo en las sesiones presenciales de la asignatura o se ausenta constantemente y/o  no demuestra una participación de manera equitativa en la presentación del caso</t>
   </si>
   <si>
-    <t>Demuestra un trabajo en equipo de manera parcial, en donde todos los miembros del equipo expresan con fluidez el conocimiento del tema expuesto, pero no todos participan de manera equitativa de las actividades planificadas en el proyecto</t>
+    <t>El estudiante realiza un mal trabajo con el equipo no fomentando un ambiente positivo, no demuestra ser participativo con su equipo en las sesiones presenciales de la asignatura o se ausenta constantemente y no demuestra una participación de manera equitativa en la presentación del caso</t>
   </si>
   <si>
-    <t>Demuestra de manera deficiente el trabajo en equipo en donde los integrantes expresan con poca fluidez y de manera imparcial el conocimiento del tema expuesto y no todos sus miembros participan de manera equitativa de las actividades planificadas en el proyecto</t>
+    <t>10. Colaboración y trabajo en equipo *</t>
   </si>
   <si>
-    <t xml:space="preserve">No demuestran un trabajo en equipo, evidenciando en su presentación la nula colaboración de alguno de sus integrantes. </t>
+    <t>2. Genera evidencias que dan cuenta del cumplimiento del Proyecto CAPSTONE, en relación a documentación, programación y almacenamiento de datos, de acuerdo a lo planificado por el equipo y que cumpla con estándares de desarrollo de la industria</t>
   </si>
   <si>
-    <t>X</t>
+    <t>Genera evidencias que dan cuenta del cumplimiento del Proyecto CAPSTONE, en relación a documentación, programación y almacenamiento de datos, de acuerdo a lo planificado por el equipo y que cumpla con estándares de desarrollo de la industria</t>
   </si>
   <si>
-    <t xml:space="preserve">Aplica la metodología definida por el equipo de acuerdo a los estándares de la disciplina, alcanzando los objetivos propuestos para el avance del proyecto. </t>
+    <t>Genera evidencias que dan cuenta del cumplimiento del Proyecto CAPSTONE, en relación a documentación, programación y almacenamiento de datos, de acuerdo a lo planificado por el equipo y no cumplen con estándares de desarrollo de la industria</t>
   </si>
   <si>
-    <t>3. Genera evidencias que dan cuenta del avance del Proyecto APT en relación a documentación, programación y almacenamiento de datos , de acuerdo a lo planificado por el equipo y que cumpla con estándares de desarrollo de la industria</t>
+    <t>Genera evidencias pero ellas no dan cuenta del cumplimiento del Proyecto CAPSTONE, en relación a documentación, programación y almacenamiento de datos, de acuerdo a lo planificado por el equipo, pero si cumple con estándares de desarrollo de la industria</t>
   </si>
   <si>
-    <t>Presenta evidencias de avance que cumplen con lo planificado por el equipo en relación a documentación, programación y almacenamiento de datos, entregando evidencias que cumplan con estándares de desarrollo que actualmente se encuentran presentes en la industria</t>
+    <t>Genera evidencias pero ellas no dan cuenta del cumplimiento del Proyecto CAPSTONE, en relación a documentación, programación y almacenamiento de datos, de acuerdo a lo planificado por el equipo, y no cumplen con estándares de desarrollo de la industria</t>
   </si>
   <si>
-    <t xml:space="preserve">Presenta evidencias de avance sin cumplir con lo planificado por el equipo en relación a documentación, programación y almacenamiento de datos, pero si sus entregas evidencian el cumplimiento de estándares de desarrollo que actualmente se encuentran presentes en la industria. </t>
+    <t>3. Relaciona el Proyecto APT con sus intereses profesionales. *</t>
   </si>
   <si>
-    <t>Presenta evidencias de avance que cumplen con lo planificado por el equipo en relación a documentación, programación y almacenamiento de datos, entregando evidencias que no cumplen con estándares de desarrollo que actualmente se encuentran presentes en la industria</t>
+    <t xml:space="preserve">Menciona los intereses profesionales y explica con claridad cómo estos se ven reflejados en el proyecto. </t>
   </si>
   <si>
-    <t>Presenta evidencias de avance sin cumplir con lo planificado por el equipo en relación a documentación, programación y almacenamiento de datos y las evidencias no cumplen con estándares de desarrollo que actualmente se encuentran presentes en la industria</t>
+    <t>Menciona los intereses profesionales, pero no queda completamente clara su conexión con el proyecto.</t>
   </si>
   <si>
-    <t>4. Utiliza de manera precisa el lenguaje técnico en los entregables de acuerdo con lo requerido por la disciplina.</t>
+    <t xml:space="preserve">Menciona los intereses profesionales sin conectarlos con el proyecto. </t>
+  </si>
+  <si>
+    <t>No menciona los intereses profesionales.</t>
+  </si>
+  <si>
+    <t>4. Relaciona el Proyecto APT con las competencias del perfil de egreso de su Plan de Estudio.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Describe una relación coherente entre el proyecto y el perfil de egreso del plan de estudio, especificando cómo debe utilizar distintas competencias para desarrollar su Proyecto APT. </t>
+  </si>
+  <si>
+    <t>Describe una relación coherente entre el proyecto y el perfil de egreso del plan de estudio, pero no especifica cómo debe utilizar distintas competencias para desarrollar su Proyecto APT.</t>
+  </si>
+  <si>
+    <t>Describe una relación que tiene elementos pero que no son coherentes entre el proyecto y el perfil de egreso del plan de estudio.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Describe una relación sin coherencia entre el proyecto y el perfil de egreso del plan de estudio o no relaciona el proyecto con el perfil de egreso. </t>
+  </si>
+  <si>
+    <t>5. Utiliza de manera precisa el lenguaje técnico en los entregables de acuerdo con lo requerido por la disciplina.</t>
   </si>
   <si>
     <t xml:space="preserve">Utiliza lenguaje técnico de su disciplina en todos los entregables de avance del proyecto. </t>
@@ -248,7 +281,7 @@
     <t xml:space="preserve">No utiliza lenguaje técnico de su disciplina en los entregables de avance del proyecto. </t>
   </si>
   <si>
-    <t>6. Entrega la documentación y evidencias requerida por la asignatura de acuerdo a la estrucutra y nombres solicitados, guardando todas las evidencias de avances en Git</t>
+    <t>7. Entrega la documentación y evidencias requerida por la asignatura de acuerdo a la estrucutra y nombres solicitados, guardando todas las evidencias de avances en Git</t>
   </si>
   <si>
     <t>Entrega la documentación y evidencias requeridas por la asignatura de acuerdo a la estrucutra y nombres solicitados, guardando todas las evidencias de avances en Git</t>
@@ -263,7 +296,13 @@
     <t>No entrega a través de Git la documentación y evidencias de avance requeridas por la asignatura</t>
   </si>
   <si>
-    <t>7.- Generan evidencias claras dentro del repositorio  del aporte de cada uno de los integrantes del equipo que permitan identificar la equidad en el trabajo y la participación de cada estudiante.</t>
+    <t>8. Expone el tema utilizando un lenguaje técnico disciplinar al presentar la propuesta y responde evidenciando un manejo de la información. *</t>
+  </si>
+  <si>
+    <t>Expone el tema utilizando un lenguaje técnico disciplinar al presentar la propuesta y responde evidenciando un manejo de la información en todo momento</t>
+  </si>
+  <si>
+    <t>9.-Generan evidencias claras dentro del repositorio  del aporte de cada uno de los integrantes del equipo que permitan identificar la equidad en el trabajo y la participación de cada estudiante.</t>
   </si>
   <si>
     <t>Generan evidencias dentro del repositorio  del proyecto del aporte de cada uno de los integrantes del equipo que permitan identificar la equidad en el trabajo y la participación de cada estudiante</t>
@@ -287,25 +326,40 @@
     <t>Edgar León</t>
   </si>
   <si>
-    <t>El Modelo de datos debe ser de lo nuevo</t>
+    <t>Comentarios PPT</t>
   </si>
   <si>
-    <t>Corregir Spanglish y ortografía</t>
+    <t>Cambiar los problemas a Oportunidad</t>
   </si>
   <si>
-    <t>El Jira no está actualizado y no refleja el estado del proyecto</t>
+    <t>Mejorar: Integración de funcionalidades?</t>
   </si>
   <si>
-    <t>El avance de lo realizado es menor de lo esperado</t>
+    <t>Separar las competencias</t>
   </si>
   <si>
-    <t>Revisar los objetivos específicos</t>
+    <t>Metodología</t>
   </si>
   <si>
-    <t>Mostraron solo que recuperar las hoteles</t>
+    <t>Cambiar roadmap y cronograma</t>
   </si>
   <si>
-    <t>Además no se ven tareas para las historias</t>
+    <t>Antes la arquitectura y luego la tecnología</t>
+  </si>
+  <si>
+    <t>Arq. Cambiar la VMs y para que es la API Tools</t>
+  </si>
+  <si>
+    <t>Slide de Prompt Engineering</t>
+  </si>
+  <si>
+    <t>Bien el sistema</t>
+  </si>
+  <si>
+    <t>Revosar rol Project Manager</t>
+  </si>
+  <si>
+    <t>El Alcance es uno solo</t>
   </si>
 </sst>
 </file>
@@ -315,7 +369,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -372,6 +426,12 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <b/>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
@@ -399,13 +459,6 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FF3B3838"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -419,25 +472,13 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="7">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -448,6 +489,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFECECEC"/>
         <bgColor rgb="FFECECEC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDEEAF6"/>
+        <bgColor rgb="FFDEEAF6"/>
       </patternFill>
     </fill>
     <fill>
@@ -470,12 +517,24 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFE2EFD9"/>
+        <bgColor rgb="FFE2EFD9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF262626"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="28">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -672,27 +731,65 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FF7F7F7F"/>
+      <left style="thin">
+        <color rgb="FF000000"/>
       </left>
-      <right style="medium">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF7F7F7F"/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
       </left>
-      <right style="medium">
-        <color rgb="FF7F7F7F"/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
       </right>
       <top/>
-      <bottom/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -713,53 +810,7 @@
       <right style="medium">
         <color rgb="FF7F7F7F"/>
       </right>
-      <top style="medium">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FF7F7F7F"/>
-      </right>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color rgb="FF7F7F7F"/>
-      </top>
       <bottom style="medium">
         <color rgb="FF7F7F7F"/>
       </bottom>
@@ -790,15 +841,33 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="medium">
+        <color rgb="FF7F7F7F"/>
+      </left>
       <right style="medium">
         <color rgb="FF7F7F7F"/>
       </right>
       <top style="medium">
         <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -806,7 +875,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -819,22 +888,25 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -843,32 +915,39 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -879,84 +958,109 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="10" fillId="8" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="14" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="9" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -989,55 +1093,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1227667</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>296333</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>35984</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>96108</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagen 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C4475985-C64F-299B-EE38-1EAF085738D5}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7133167" y="6572250"/>
-          <a:ext cx="7772400" cy="5334858"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1336,11 +1391,279 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B396D1B-8A63-4A90-BA20-D34AC13A3962}">
+  <dimension ref="A1:F13"/>
+  <sheetViews>
+    <sheetView topLeftCell="A5" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="6" width="38.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="51" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="51" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="51"/>
+      <c r="B2" s="52" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="52" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="51"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="51"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="37">
+        <v>-0.3</v>
+      </c>
+      <c r="E3" s="37">
+        <v>0</v>
+      </c>
+      <c r="F3" s="51"/>
+    </row>
+    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.2">
+      <c r="A4" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" s="39">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="75" x14ac:dyDescent="0.2">
+      <c r="A5" s="42" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="38" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="38" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5" s="39">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="31" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="42" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="38" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6" s="39">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="60" x14ac:dyDescent="0.2">
+      <c r="A7" s="43" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" s="44" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="44" t="s">
+        <v>56</v>
+      </c>
+      <c r="D7" s="44" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7" s="45" t="s">
+        <v>58</v>
+      </c>
+      <c r="F7" s="39">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.2">
+      <c r="A8" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="38" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="E8" s="38" t="s">
+        <v>63</v>
+      </c>
+      <c r="F8" s="39">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.2">
+      <c r="A9" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="39">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="60" x14ac:dyDescent="0.2">
+      <c r="A10" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="D10" s="38" t="s">
+        <v>67</v>
+      </c>
+      <c r="E10" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="F10" s="39">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="61" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="46" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="47" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" s="39">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="61" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="48" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12" s="49" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" s="49" t="s">
+        <v>73</v>
+      </c>
+      <c r="D12" s="49" t="s">
+        <v>74</v>
+      </c>
+      <c r="E12" s="49" t="s">
+        <v>75</v>
+      </c>
+      <c r="F12" s="50">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="91" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="F13" s="39">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:F3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:K895"/>
+  <dimension ref="A2:K926"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C70" sqref="C70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -1359,6 +1682,12 @@
   <sheetData>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C2" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="E2" s="68">
         <v>1</v>
       </c>
     </row>
@@ -1366,564 +1695,1271 @@
       <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="40" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="D3" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="54"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>1</v>
       </c>
-      <c r="B4" s="40" t="s">
-        <v>63</v>
+      <c r="B4" s="28" t="s">
+        <v>76</v>
       </c>
       <c r="C4" s="5">
-        <f>EVALUACION2!$C$22</f>
-        <v>5.0999999999999996</v>
+        <f>EVALUACION1!$C$21</f>
+        <v>6</v>
+      </c>
+      <c r="D4" s="5">
+        <f>$C$32</f>
+        <v>7</v>
+      </c>
+      <c r="E4" s="6">
+        <f>C4*C$2+D4*D$2</f>
+        <v>6.25</v>
       </c>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>2</v>
       </c>
-      <c r="B5" s="40" t="s">
-        <v>64</v>
+      <c r="B5" s="28" t="s">
+        <v>77</v>
       </c>
       <c r="C5" s="5">
-        <f>EVALUACION2!$C$22</f>
-        <v>5.0999999999999996</v>
+        <f>EVALUACION1!$C$21</f>
+        <v>6</v>
+      </c>
+      <c r="D5" s="5">
+        <f>C44</f>
+        <v>7</v>
+      </c>
+      <c r="E5" s="6">
+        <f t="shared" ref="E5:E6" si="0">C5*C$2+D5*D$2</f>
+        <v>6.25</v>
       </c>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>3</v>
       </c>
-      <c r="B6" s="40" t="s">
-        <v>65</v>
+      <c r="B6" s="28" t="s">
+        <v>78</v>
       </c>
       <c r="C6" s="5">
-        <f>EVALUACION2!$C$22</f>
-        <v>5.0999999999999996</v>
+        <f>EVALUACION1!$C$21</f>
+        <v>6</v>
+      </c>
+      <c r="D6" s="5">
+        <f>C55</f>
+        <v>7</v>
+      </c>
+      <c r="E6" s="6">
+        <f t="shared" si="0"/>
+        <v>6.25</v>
       </c>
       <c r="G6" s="1"/>
     </row>
     <row r="11" spans="1:11" ht="19" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="41" t="s">
+      <c r="A11" s="69" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="14"/>
-      <c r="C11" s="45" t="s">
+      <c r="B11" s="15"/>
+      <c r="C11" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="46" t="s">
+      <c r="D11" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="48"/>
-      <c r="F11" s="48"/>
-      <c r="G11" s="48"/>
-      <c r="H11" s="48"/>
-      <c r="I11" s="48"/>
-      <c r="J11" s="48"/>
-      <c r="K11" s="47"/>
+      <c r="E11" s="67"/>
+      <c r="F11" s="67"/>
+      <c r="G11" s="67"/>
+      <c r="H11" s="67"/>
+      <c r="I11" s="67"/>
+      <c r="J11" s="67"/>
+      <c r="K11" s="63"/>
     </row>
     <row r="12" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="42"/>
-      <c r="B12" s="20" t="s">
+      <c r="A12" s="65"/>
+      <c r="B12" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="44"/>
-      <c r="D12" s="46" t="s">
+      <c r="C12" s="54"/>
+      <c r="D12" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="E12" s="47"/>
-      <c r="F12" s="46" t="s">
+      <c r="E12" s="63"/>
+      <c r="F12" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="G12" s="47"/>
-      <c r="H12" s="49" t="s">
-        <v>23</v>
-      </c>
-      <c r="I12" s="47"/>
-      <c r="J12" s="46" t="s">
+      <c r="G12" s="63"/>
+      <c r="H12" s="66" t="s">
+        <v>27</v>
+      </c>
+      <c r="I12" s="63"/>
+      <c r="J12" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="K12" s="47"/>
-    </row>
-    <row r="13" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="43"/>
-      <c r="B13" s="27" t="str">
+      <c r="K12" s="63"/>
+    </row>
+    <row r="13" spans="1:11" ht="26" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="70"/>
+      <c r="B13" s="31" t="str">
         <f>RUBRICA!A4</f>
-        <v xml:space="preserve">1. Propone ajustes al Proyecto APT considerando dificultades, facilitadores y retroalimentación. </v>
-      </c>
-      <c r="C13" s="25" t="s">
+        <v>1. Implementa una metodología que permite el logro de los objetivos propuestos, de acuerdo a los estándares de la disciplina.</v>
+      </c>
+      <c r="C13" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="15" t="str">
-        <f t="shared" ref="D13:D17" si="0">IF($C13=CL,"X","")</f>
+      <c r="D13" s="17" t="str">
+        <f t="shared" ref="D13:D16" si="1">IF($C13=CL,"X","")</f>
         <v>X</v>
       </c>
-      <c r="E13" s="15">
+      <c r="E13" s="17">
         <f>IF(D13="X",100*0.1,"")</f>
         <v>10</v>
       </c>
-      <c r="F13" s="15" t="str">
-        <f t="shared" ref="F13:F17" si="1">IF($C13=L,"X","")</f>
+      <c r="F13" s="17" t="str">
+        <f t="shared" ref="F13:F16" si="2">IF($C13=L,"X","")</f>
         <v/>
       </c>
-      <c r="G13" s="15" t="str">
+      <c r="G13" s="17" t="str">
         <f>IF(F13="X",60*0.1,"")</f>
         <v/>
       </c>
-      <c r="H13" s="15" t="str">
-        <f t="shared" ref="H13:H17" si="2">IF($C13=ML,"X","")</f>
+      <c r="H13" s="17" t="str">
+        <f t="shared" ref="H13:H16" si="3">IF($C13=ML,"X","")</f>
         <v/>
       </c>
-      <c r="I13" s="15" t="str">
+      <c r="I13" s="17" t="str">
         <f>IF(H13="X",30*0.1,"")</f>
         <v/>
       </c>
-      <c r="J13" s="15" t="str">
-        <f t="shared" ref="J13:J17" si="3">IF($C13=NL,"X","")</f>
+      <c r="J13" s="17" t="str">
+        <f t="shared" ref="J13:J16" si="4">IF($C13=NL,"X","")</f>
         <v/>
       </c>
-      <c r="K13" s="15" t="str">
-        <f t="shared" ref="K13:K17" si="4">IF($J13="X",0,"")</f>
+      <c r="K13" s="17" t="str">
+        <f t="shared" ref="K13:K16" si="5">IF($J13="X",0,"")</f>
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="26.5" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="43"/>
-      <c r="B14" s="27" t="str">
+    <row r="14" spans="1:11" ht="39" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="70"/>
+      <c r="B14" s="31" t="str">
         <f>RUBRICA!A5</f>
-        <v>2. Aplica una metodología que permite el logro de los objetivos propuestos, de acuerdo a los estándares de la disciplina.</v>
-      </c>
-      <c r="C14" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" s="15" t="str">
-        <f t="shared" si="0"/>
-        <v>X</v>
-      </c>
-      <c r="E14" s="15">
-        <f>IF(D14="X",100*0.1,"")</f>
-        <v>10</v>
-      </c>
-      <c r="F14" s="15" t="str">
+        <v>2. Genera evidencias que dan cuenta del cumplimiento del Proyecto CAPSTONE, en relación a documentación, programación y almacenamiento de datos, de acuerdo a lo planificado por el equipo y que cumpla con estándares de desarrollo de la industria</v>
+      </c>
+      <c r="C14" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="17" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G14" s="15" t="str">
-        <f>IF(F14="X",60*0.1,"")</f>
+      <c r="E14" s="17" t="str">
+        <f>IF(D14="X",100*0.2,"")</f>
         <v/>
       </c>
-      <c r="H14" s="15" t="str">
+      <c r="F14" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>X</v>
+      </c>
+      <c r="G14" s="17">
+        <f>IF(F14="X",60*0.2,"")</f>
+        <v>12</v>
+      </c>
+      <c r="H14" s="17" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I14" s="17" t="str">
+        <f>IF(H14="X",30*0.2,"")</f>
+        <v/>
+      </c>
+      <c r="J14" s="17" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="K14" s="17" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="70"/>
+      <c r="B15" s="31" t="str">
+        <f>RUBRICA!A7</f>
+        <v>4. Relaciona el Proyecto APT con las competencias del perfil de egreso de su Plan de Estudio.</v>
+      </c>
+      <c r="C15" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>X</v>
+      </c>
+      <c r="E15" s="17">
+        <f>IF(D15="X",100*0.05,"")</f>
+        <v>5</v>
+      </c>
+      <c r="F15" s="17" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="I14" s="15" t="str">
-        <f>IF(H14="X",30*0.1,"")</f>
+      <c r="G15" s="17" t="str">
+        <f>IF(F15="X",60*0.05,"")</f>
         <v/>
       </c>
-      <c r="J14" s="15" t="str">
+      <c r="H15" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="K14" s="15" t="str">
+      <c r="I15" s="17" t="str">
+        <f>IF(H15="X",30*0.05,"")</f>
+        <v/>
+      </c>
+      <c r="J15" s="17" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-    </row>
-    <row r="15" spans="1:11" ht="39" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="43"/>
-      <c r="B15" s="27" t="str">
-        <f>RUBRICA!A6</f>
-        <v>3. Genera evidencias que dan cuenta del avance del Proyecto APT en relación a documentación, programación y almacenamiento de datos , de acuerdo a lo planificado por el equipo y que cumpla con estándares de desarrollo de la industria</v>
-      </c>
-      <c r="C15" s="25" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" s="15" t="str">
-        <f t="shared" si="0"/>
+      <c r="K15" s="17" t="str">
+        <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="E15" s="15" t="str">
-        <f>IF(D15="X",100*0.25,"")</f>
-        <v/>
-      </c>
-      <c r="F15" s="15" t="str">
+    </row>
+    <row r="16" spans="1:11" ht="26" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="70"/>
+      <c r="B16" s="31" t="str">
+        <f>RUBRICA!A8</f>
+        <v>5. Utiliza de manera precisa el lenguaje técnico en los entregables de acuerdo con lo requerido por la disciplina.</v>
+      </c>
+      <c r="C16" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="17" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G15" s="15" t="str">
-        <f>IF(F15="X",60*0.25,"")</f>
+      <c r="E16" s="17" t="str">
+        <f>IF(D16="X",100*0.05,"")</f>
         <v/>
       </c>
-      <c r="H15" s="15" t="str">
+      <c r="F16" s="17" t="str">
         <f t="shared" si="2"/>
         <v>X</v>
       </c>
-      <c r="I15" s="15">
-        <f>IF(H15="X",30*0.25,"")</f>
-        <v>7.5</v>
-      </c>
-      <c r="J15" s="15" t="str">
+      <c r="G16" s="17">
+        <f>IF(F16="X",60*0.05,"")</f>
+        <v>3</v>
+      </c>
+      <c r="H16" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="K15" s="15" t="str">
+      <c r="I16" s="17" t="str">
+        <f>IF(H16="X",30*0.05,"")</f>
+        <v/>
+      </c>
+      <c r="J16" s="17" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-    </row>
-    <row r="16" spans="1:11" ht="26" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="43"/>
-      <c r="B16" s="27" t="str">
-        <f>RUBRICA!A7</f>
-        <v>4. Utiliza de manera precisa el lenguaje técnico en los entregables de acuerdo con lo requerido por la disciplina.</v>
-      </c>
-      <c r="C16" s="25" t="s">
+      <c r="K16" s="17" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="26" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="70"/>
+      <c r="B17" s="31" t="str">
+        <f>RUBRICA!A9</f>
+        <v xml:space="preserve">6. Utiliza correctamente las reglas de redacción, ortografía (literal, puntual, acentual) y las normas para citas y referencias. </v>
+      </c>
+      <c r="C17" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="15" t="str">
-        <f t="shared" si="0"/>
+      <c r="D17" s="17" t="str">
+        <f>IF($C17=CL,"X","")</f>
         <v>X</v>
       </c>
-      <c r="E16" s="15">
-        <f>IF(D16="X",100*0.05,"")</f>
-        <v>5</v>
-      </c>
-      <c r="F16" s="15" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="G16" s="15" t="str">
-        <f>IF(F16="X",60*0.05,"")</f>
-        <v/>
-      </c>
-      <c r="H16" s="15" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="I16" s="15" t="str">
-        <f>IF(H16="X",30*0.05,"")</f>
-        <v/>
-      </c>
-      <c r="J16" s="15" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="K16" s="15" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-    </row>
-    <row r="17" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="43"/>
-      <c r="B17" s="27" t="str">
-        <f>RUBRICA!A8</f>
-        <v xml:space="preserve">5. Utiliza reglas de redacción, ortografía (literal, puntual, acentual) y las normas para citas y referencias. </v>
-      </c>
-      <c r="C17" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" s="15" t="str">
-        <f t="shared" si="0"/>
-        <v>X</v>
-      </c>
-      <c r="E17" s="15">
+      <c r="E17" s="17">
         <f>IF(D17="X",100*0.05,"")</f>
         <v>5</v>
       </c>
-      <c r="F17" s="15" t="str">
-        <f t="shared" si="1"/>
+      <c r="F17" s="17" t="str">
+        <f>IF($C17=L,"X","")</f>
         <v/>
       </c>
-      <c r="G17" s="15" t="str">
+      <c r="G17" s="17" t="str">
         <f>IF(F17="X",60*0.05,"")</f>
         <v/>
       </c>
-      <c r="H17" s="15" t="str">
-        <f t="shared" si="2"/>
+      <c r="H17" s="17" t="str">
+        <f>IF($C17=ML,"X","")</f>
         <v/>
       </c>
-      <c r="I17" s="15" t="str">
+      <c r="I17" s="17" t="str">
         <f>IF(H17="X",30*0.05,"")</f>
         <v/>
       </c>
-      <c r="J17" s="15" t="str">
-        <f t="shared" si="3"/>
+      <c r="J17" s="17" t="str">
+        <f>IF($C17=NL,"X","")</f>
         <v/>
       </c>
-      <c r="K17" s="15" t="str">
-        <f t="shared" si="4"/>
+      <c r="K17" s="17" t="str">
+        <f t="shared" ref="K17:K19" si="6">IF($J17="X",0,"")</f>
         <v/>
       </c>
     </row>
     <row r="18" spans="1:11" ht="26" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="43"/>
-      <c r="B18" s="27" t="str">
-        <f>RUBRICA!A9</f>
-        <v>6. Entrega la documentación y evidencias requerida por la asignatura de acuerdo a la estrucutra y nombres solicitados, guardando todas las evidencias de avances en Git</v>
-      </c>
-      <c r="C18" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" s="15" t="str">
+      <c r="A18" s="70"/>
+      <c r="B18" s="31" t="str">
+        <f>RUBRICA!A10</f>
+        <v>7. Entrega la documentación y evidencias requerida por la asignatura de acuerdo a la estrucutra y nombres solicitados, guardando todas las evidencias de avances en Git</v>
+      </c>
+      <c r="C18" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="17" t="str">
         <f>IF($C18=CL,"X","")</f>
+        <v>X</v>
+      </c>
+      <c r="E18" s="17">
+        <f>IF(D18="X",100*0.15,"")</f>
+        <v>15</v>
+      </c>
+      <c r="F18" s="17" t="str">
+        <f>IF($C18=L,"X","")</f>
         <v/>
       </c>
-      <c r="E18" s="15" t="str">
-        <f>IF(D18="X",100*0.2,"")</f>
+      <c r="G18" s="17" t="str">
+        <f>IF(F18="X",60*0.15,"")</f>
         <v/>
       </c>
-      <c r="F18" s="15" t="str">
-        <f>IF($C18=L,"X","")</f>
-        <v>X</v>
-      </c>
-      <c r="G18" s="15">
-        <f>IF(F18="X",60*0.2,"")</f>
-        <v>12</v>
-      </c>
-      <c r="H18" s="15" t="str">
+      <c r="H18" s="17" t="str">
         <f>IF($C18=ML,"X","")</f>
         <v/>
       </c>
-      <c r="I18" s="15" t="str">
-        <f>IF(H18="X",30*0.2,"")</f>
+      <c r="I18" s="17" t="str">
+        <f>IF(H18="X",30*0.15,"")</f>
         <v/>
       </c>
-      <c r="J18" s="15" t="str">
+      <c r="J18" s="17" t="str">
         <f>IF($C18=NL,"X","")</f>
         <v/>
       </c>
-      <c r="K18" s="15" t="str">
-        <f t="shared" ref="K18:K20" si="5">IF($J18="X",0,"")</f>
+      <c r="K18" s="17" t="str">
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="26" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="43"/>
-      <c r="B19" s="27" t="str">
-        <f>RUBRICA!A10</f>
-        <v>7.- Generan evidencias claras dentro del repositorio  del aporte de cada uno de los integrantes del equipo que permitan identificar la equidad en el trabajo y la participación de cada estudiante.</v>
-      </c>
-      <c r="C19" s="25" t="s">
+    <row r="19" spans="1:11" ht="22.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="70"/>
+      <c r="B19" s="31" t="str">
+        <f>RUBRICA!A12</f>
+        <v>9.-Generan evidencias claras dentro del repositorio  del aporte de cada uno de los integrantes del equipo que permitan identificar la equidad en el trabajo y la participación de cada estudiante.</v>
+      </c>
+      <c r="C19" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="D19" s="15" t="str">
+      <c r="D19" s="17" t="str">
         <f>IF($C19=CL,"X","")</f>
         <v>X</v>
       </c>
-      <c r="E19" s="15">
+      <c r="E19" s="17">
         <f>IF(D19="X",100*0.15,"")</f>
         <v>15</v>
       </c>
-      <c r="F19" s="15" t="str">
+      <c r="F19" s="17" t="str">
         <f>IF($C19=L,"X","")</f>
         <v/>
       </c>
-      <c r="G19" s="15" t="str">
+      <c r="G19" s="17" t="str">
         <f>IF(F19="X",60*0.15,"")</f>
         <v/>
       </c>
-      <c r="H19" s="15" t="str">
+      <c r="H19" s="17" t="str">
         <f>IF($C19=ML,"X","")</f>
         <v/>
       </c>
-      <c r="I19" s="15" t="str">
+      <c r="I19" s="17" t="str">
         <f>IF(H19="X",30*0.15,"")</f>
         <v/>
       </c>
-      <c r="J19" s="15" t="str">
+      <c r="J19" s="17" t="str">
         <f>IF($C19=NL,"X","")</f>
         <v/>
       </c>
-      <c r="K19" s="15" t="str">
-        <f t="shared" si="5"/>
+      <c r="K19" s="17" t="str">
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="26" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="43"/>
-      <c r="B20" s="27" t="str">
+    <row r="20" spans="1:11" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="65"/>
+      <c r="B20" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="34">
+        <f>E20+G20+I20+K20</f>
+        <v>65</v>
+      </c>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20">
+        <f>SUM(E13:E19)</f>
+        <v>50</v>
+      </c>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20">
+        <f>SUM(G13:G19)</f>
+        <v>15</v>
+      </c>
+      <c r="H20" s="20"/>
+      <c r="I20" s="20">
+        <f>SUM(I13:I19)</f>
+        <v>0</v>
+      </c>
+      <c r="J20" s="20"/>
+      <c r="K20" s="20">
+        <f>SUM(K13:K19)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="54"/>
+      <c r="B21" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="21">
+        <f>VLOOKUP(C20,ESCALA_IEP!A1:B152,2,FALSE)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="64" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24" s="53" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" s="56" t="str">
+        <f>$B$4</f>
+        <v>José Tobar Estay</v>
+      </c>
+      <c r="D24" s="57"/>
+      <c r="E24" s="57"/>
+      <c r="F24" s="57"/>
+      <c r="G24" s="57"/>
+      <c r="H24" s="57"/>
+      <c r="I24" s="57"/>
+      <c r="J24" s="57"/>
+      <c r="K24" s="58"/>
+    </row>
+    <row r="25" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="65"/>
+      <c r="B25" s="54"/>
+      <c r="C25" s="59"/>
+      <c r="D25" s="60"/>
+      <c r="E25" s="60"/>
+      <c r="F25" s="60"/>
+      <c r="G25" s="60"/>
+      <c r="H25" s="60"/>
+      <c r="I25" s="60"/>
+      <c r="J25" s="60"/>
+      <c r="K25" s="61"/>
+    </row>
+    <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="65"/>
+      <c r="B26" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" s="55" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" s="62" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" s="67"/>
+      <c r="F26" s="67"/>
+      <c r="G26" s="67"/>
+      <c r="H26" s="67"/>
+      <c r="I26" s="67"/>
+      <c r="J26" s="67"/>
+      <c r="K26" s="63"/>
+    </row>
+    <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="65"/>
+      <c r="B27" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" s="54"/>
+      <c r="D27" s="62" t="s">
+        <v>5</v>
+      </c>
+      <c r="E27" s="63"/>
+      <c r="F27" s="62" t="s">
+        <v>6</v>
+      </c>
+      <c r="G27" s="63"/>
+      <c r="H27" s="66" t="s">
+        <v>27</v>
+      </c>
+      <c r="I27" s="63"/>
+      <c r="J27" s="62" t="s">
+        <v>7</v>
+      </c>
+      <c r="K27" s="63"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28" s="65"/>
+      <c r="B28" s="31" t="str">
+        <f>RUBRICA!A6</f>
+        <v>3. Relaciona el Proyecto APT con sus intereses profesionales. *</v>
+      </c>
+      <c r="C28" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28" s="17" t="str">
+        <f t="shared" ref="D28:D30" si="7">IF($C28=CL,"X","")</f>
+        <v>X</v>
+      </c>
+      <c r="E28" s="17">
+        <f>IF(D28="X",100*0.05,"")</f>
+        <v>5</v>
+      </c>
+      <c r="F28" s="17" t="str">
+        <f t="shared" ref="F28:F30" si="8">IF($C28=L,"X","")</f>
+        <v/>
+      </c>
+      <c r="G28" s="17" t="str">
+        <f>IF(F28="X",60*0.05,"")</f>
+        <v/>
+      </c>
+      <c r="H28" s="17" t="str">
+        <f t="shared" ref="H28:H30" si="9">IF($C28=ML,"X","")</f>
+        <v/>
+      </c>
+      <c r="I28" s="17" t="str">
+        <f>IF(H28="X",30*0.05,"")</f>
+        <v/>
+      </c>
+      <c r="J28" s="17" t="str">
+        <f t="shared" ref="J28:J30" si="10">IF($C28=NL,"X","")</f>
+        <v/>
+      </c>
+      <c r="K28" s="17" t="str">
+        <f t="shared" ref="K28:K30" si="11">IF($J28="X",0,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="24.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="65"/>
+      <c r="B29" s="31" t="str">
         <f>RUBRICA!A11</f>
-        <v>8. Demuestra un trabajo en equipo en donde todos los miembros del equipo expresan con fluidez el conocimiento del tema expuesto y  participan de las actividades planificadas en el proyecto</v>
-      </c>
-      <c r="C20" s="25" t="s">
+        <v>8. Expone el tema utilizando un lenguaje técnico disciplinar al presentar la propuesta y responde evidenciando un manejo de la información. *</v>
+      </c>
+      <c r="C29" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="D20" s="15" t="str">
-        <f>IF($C20=CL,"X","")</f>
+      <c r="D29" s="17" t="str">
+        <f t="shared" si="7"/>
         <v>X</v>
       </c>
-      <c r="E20" s="15">
-        <f>IF(D20="X",100*0.1,"")</f>
+      <c r="E29" s="17">
+        <f>IF(D29="X",100*0.1,"")</f>
         <v>10</v>
       </c>
-      <c r="F20" s="15" t="str">
-        <f>IF($C20=L,"X","")</f>
+      <c r="F29" s="17" t="str">
+        <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="G20" s="15" t="str">
-        <f>IF(F20="X",60*0.1,"")</f>
+      <c r="G29" s="17" t="str">
+        <f>IF(F29="X",60*0.1,"")</f>
         <v/>
       </c>
-      <c r="H20" s="15" t="str">
-        <f>IF($C20=ML,"X","")</f>
+      <c r="H29" s="17" t="str">
+        <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="I20" s="15" t="str">
-        <f>IF(H20="X",30*0.1,"")</f>
+      <c r="I29" s="17" t="str">
+        <f>IF(H29="X",30*0.1,"")</f>
         <v/>
       </c>
-      <c r="J20" s="15" t="str">
-        <f>IF($C20=NL,"X","")</f>
+      <c r="J29" s="17" t="str">
+        <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="K20" s="15" t="str">
-        <f t="shared" si="5"/>
+      <c r="K29" s="17" t="str">
+        <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="42"/>
-      <c r="B21" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="C21" s="30">
-        <f>E21+G21+I21+K21</f>
-        <v>74.5</v>
-      </c>
-      <c r="D21" s="16"/>
-      <c r="E21" s="16">
-        <f>SUM(E13:E20)</f>
-        <v>55</v>
-      </c>
-      <c r="F21" s="16"/>
-      <c r="G21" s="16">
-        <f>SUM(G13:G20)</f>
+    <row r="30" spans="1:11" ht="25.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="65"/>
+      <c r="B30" s="31" t="str">
+        <f>RUBRICA!A13</f>
+        <v>10. Colaboración y trabajo en equipo *</v>
+      </c>
+      <c r="C30" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30" s="17" t="str">
+        <f t="shared" si="7"/>
+        <v>X</v>
+      </c>
+      <c r="E30" s="17">
+        <f>IF(D30="X",100*0.1,"")</f>
+        <v>10</v>
+      </c>
+      <c r="F30" s="17" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="G30" s="17" t="str">
+        <f>IF(F30="X",60*0.1,"")</f>
+        <v/>
+      </c>
+      <c r="H30" s="17" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="I30" s="17" t="str">
+        <f>IF(H30="X",30*0.1,"")</f>
+        <v/>
+      </c>
+      <c r="J30" s="17" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="K30" s="17" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="65"/>
+      <c r="B31" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" s="19">
+        <f>E31+G31+I31+K31</f>
+        <v>25</v>
+      </c>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20">
+        <f>SUM(E28:E30)</f>
+        <v>25</v>
+      </c>
+      <c r="F31" s="20"/>
+      <c r="G31" s="20">
+        <f>SUM(G28:G30)</f>
+        <v>0</v>
+      </c>
+      <c r="H31" s="20"/>
+      <c r="I31" s="20">
+        <f>SUM(I28:I30)</f>
+        <v>0</v>
+      </c>
+      <c r="J31" s="20"/>
+      <c r="K31" s="20">
+        <f>SUM(K29:K30)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="54"/>
+      <c r="B32" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C32" s="21">
+        <f>VLOOKUP(C31,ESCALA_TRAB_EQUIP!A1:B52,2,FALSE)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="23"/>
+      <c r="C33" s="24"/>
+    </row>
+    <row r="34" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="23"/>
+      <c r="C34" s="24"/>
+    </row>
+    <row r="35" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="36" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="64" t="s">
+        <v>15</v>
+      </c>
+      <c r="B36" s="53" t="s">
+        <v>16</v>
+      </c>
+      <c r="C36" s="56" t="str">
+        <f>B5</f>
+        <v>Cristóbal Cabezas Espinoza</v>
+      </c>
+      <c r="D36" s="57"/>
+      <c r="E36" s="57"/>
+      <c r="F36" s="57"/>
+      <c r="G36" s="57"/>
+      <c r="H36" s="57"/>
+      <c r="I36" s="57"/>
+      <c r="J36" s="57"/>
+      <c r="K36" s="58"/>
+    </row>
+    <row r="37" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="65"/>
+      <c r="B37" s="54"/>
+      <c r="C37" s="59"/>
+      <c r="D37" s="60"/>
+      <c r="E37" s="60"/>
+      <c r="F37" s="60"/>
+      <c r="G37" s="60"/>
+      <c r="H37" s="60"/>
+      <c r="I37" s="60"/>
+      <c r="J37" s="60"/>
+      <c r="K37" s="61"/>
+    </row>
+    <row r="38" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="65"/>
+      <c r="B38" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C38" s="55" t="s">
+        <v>10</v>
+      </c>
+      <c r="D38" s="62" t="s">
+        <v>11</v>
+      </c>
+      <c r="E38" s="67"/>
+      <c r="F38" s="67"/>
+      <c r="G38" s="67"/>
+      <c r="H38" s="67"/>
+      <c r="I38" s="67"/>
+      <c r="J38" s="67"/>
+      <c r="K38" s="63"/>
+    </row>
+    <row r="39" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="65"/>
+      <c r="B39" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="H21" s="16"/>
-      <c r="I21" s="16">
-        <f>SUM(I13:I20)</f>
-        <v>7.5</v>
-      </c>
-      <c r="J21" s="16"/>
-      <c r="K21" s="16">
-        <f>SUM(K13:K20)</f>
+      <c r="C39" s="54"/>
+      <c r="D39" s="62" t="s">
+        <v>5</v>
+      </c>
+      <c r="E39" s="63"/>
+      <c r="F39" s="62" t="s">
+        <v>6</v>
+      </c>
+      <c r="G39" s="63"/>
+      <c r="H39" s="66" t="s">
+        <v>27</v>
+      </c>
+      <c r="I39" s="63"/>
+      <c r="J39" s="62" t="s">
+        <v>7</v>
+      </c>
+      <c r="K39" s="63"/>
+    </row>
+    <row r="40" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="65"/>
+      <c r="B40" s="31" t="str">
+        <f>RUBRICA!A6</f>
+        <v>3. Relaciona el Proyecto APT con sus intereses profesionales. *</v>
+      </c>
+      <c r="C40" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="D40" s="17" t="str">
+        <f t="shared" ref="D40:D42" si="12">IF($C40=CL,"X","")</f>
+        <v>X</v>
+      </c>
+      <c r="E40" s="17">
+        <f>IF(D40="X",100*0.05,"")</f>
+        <v>5</v>
+      </c>
+      <c r="F40" s="17" t="str">
+        <f t="shared" ref="F40:F42" si="13">IF($C40=L,"X","")</f>
+        <v/>
+      </c>
+      <c r="G40" s="17" t="str">
+        <f>IF(F40="X",60*0.05,"")</f>
+        <v/>
+      </c>
+      <c r="H40" s="17" t="str">
+        <f t="shared" ref="H40:H42" si="14">IF($C40=ML,"X","")</f>
+        <v/>
+      </c>
+      <c r="I40" s="17" t="str">
+        <f>IF(H40="X",30*0.05,"")</f>
+        <v/>
+      </c>
+      <c r="J40" s="17" t="str">
+        <f t="shared" ref="J40:J42" si="15">IF($C40=NL,"X","")</f>
+        <v/>
+      </c>
+      <c r="K40" s="17" t="str">
+        <f t="shared" ref="K40:K42" si="16">IF($J40="X",0,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="25.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="65"/>
+      <c r="B41" s="31" t="str">
+        <f>RUBRICA!A11</f>
+        <v>8. Expone el tema utilizando un lenguaje técnico disciplinar al presentar la propuesta y responde evidenciando un manejo de la información. *</v>
+      </c>
+      <c r="C41" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="D41" s="17" t="str">
+        <f t="shared" si="12"/>
+        <v>X</v>
+      </c>
+      <c r="E41" s="17">
+        <f>IF(D41="X",100*0.1,"")</f>
+        <v>10</v>
+      </c>
+      <c r="F41" s="17" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="G41" s="17" t="str">
+        <f>IF(F41="X",60*0.1,"")</f>
+        <v/>
+      </c>
+      <c r="H41" s="17" t="str">
+        <f t="shared" si="14"/>
+        <v/>
+      </c>
+      <c r="I41" s="17" t="str">
+        <f>IF(H41="X",30*0.1,"")</f>
+        <v/>
+      </c>
+      <c r="J41" s="17" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+      <c r="K41" s="17" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A42" s="65"/>
+      <c r="B42" s="31" t="str">
+        <f>RUBRICA!A13</f>
+        <v>10. Colaboración y trabajo en equipo *</v>
+      </c>
+      <c r="C42" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="D42" s="17" t="str">
+        <f t="shared" si="12"/>
+        <v>X</v>
+      </c>
+      <c r="E42" s="17">
+        <f>IF(D42="X",100*0.1,"")</f>
+        <v>10</v>
+      </c>
+      <c r="F42" s="17" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="G42" s="17" t="str">
+        <f>IF(F42="X",60*0.1,"")</f>
+        <v/>
+      </c>
+      <c r="H42" s="17" t="str">
+        <f t="shared" si="14"/>
+        <v/>
+      </c>
+      <c r="I42" s="17" t="str">
+        <f>IF(H42="X",30*0.1,"")</f>
+        <v/>
+      </c>
+      <c r="J42" s="17" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+      <c r="K42" s="17" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="65"/>
+      <c r="B43" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="C43" s="19">
+        <f>E43+G43+I43+K43</f>
+        <v>25</v>
+      </c>
+      <c r="D43" s="20"/>
+      <c r="E43" s="20">
+        <f>SUM(E40:E42)</f>
+        <v>25</v>
+      </c>
+      <c r="F43" s="20"/>
+      <c r="G43" s="20">
+        <f>SUM(G40:G42)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="44"/>
-      <c r="B22" s="29" t="s">
+      <c r="H43" s="20"/>
+      <c r="I43" s="20">
+        <f>SUM(I40:I42)</f>
+        <v>0</v>
+      </c>
+      <c r="J43" s="20"/>
+      <c r="K43" s="20">
+        <f>SUM(K41:K42)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="54"/>
+      <c r="B44" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="17">
-        <f>VLOOKUP(C21,ESCALA_IEP!A2:B202,2,FALSE)</f>
-        <v>5.0999999999999996</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D23" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="33"/>
-    </row>
-    <row r="25" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="18"/>
-      <c r="C25" s="19"/>
-    </row>
-    <row r="26" spans="1:11" ht="31.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="34"/>
-    </row>
-    <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="39" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="39" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="39" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="39" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="33" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="39" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="34" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="39" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="35" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="36" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="37" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="38" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="39" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="40" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="41" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="42" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="43" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="44" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="45" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="46" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="47" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="48" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="51" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="52" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="53" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="54" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="55" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="56" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="57" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="58" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="59" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="60" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="61" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="62" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="63" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="64" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="65" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="66" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="67" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="68" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="69" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="70" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="71" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="72" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="73" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="74" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="76" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="77" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="78" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="79" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="80" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="C44" s="21">
+        <f>VLOOKUP(C43,ESCALA_TRAB_EQUIP!A1:B52,2,FALSE)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="23"/>
+      <c r="C45" s="24"/>
+    </row>
+    <row r="46" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="23"/>
+      <c r="C46" s="24"/>
+    </row>
+    <row r="47" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="64" t="s">
+        <v>15</v>
+      </c>
+      <c r="B47" s="53" t="s">
+        <v>16</v>
+      </c>
+      <c r="C47" s="56" t="str">
+        <f>B6</f>
+        <v>Edgar León</v>
+      </c>
+      <c r="D47" s="57"/>
+      <c r="E47" s="57"/>
+      <c r="F47" s="57"/>
+      <c r="G47" s="57"/>
+      <c r="H47" s="57"/>
+      <c r="I47" s="57"/>
+      <c r="J47" s="57"/>
+      <c r="K47" s="58"/>
+    </row>
+    <row r="48" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="65"/>
+      <c r="B48" s="54"/>
+      <c r="C48" s="59"/>
+      <c r="D48" s="60"/>
+      <c r="E48" s="60"/>
+      <c r="F48" s="60"/>
+      <c r="G48" s="60"/>
+      <c r="H48" s="60"/>
+      <c r="I48" s="60"/>
+      <c r="J48" s="60"/>
+      <c r="K48" s="61"/>
+    </row>
+    <row r="49" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="65"/>
+      <c r="B49" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C49" s="55" t="s">
+        <v>10</v>
+      </c>
+      <c r="D49" s="62" t="s">
+        <v>11</v>
+      </c>
+      <c r="E49" s="67"/>
+      <c r="F49" s="67"/>
+      <c r="G49" s="67"/>
+      <c r="H49" s="67"/>
+      <c r="I49" s="67"/>
+      <c r="J49" s="67"/>
+      <c r="K49" s="63"/>
+    </row>
+    <row r="50" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="65"/>
+      <c r="B50" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C50" s="54"/>
+      <c r="D50" s="62" t="s">
+        <v>5</v>
+      </c>
+      <c r="E50" s="63"/>
+      <c r="F50" s="62" t="s">
+        <v>6</v>
+      </c>
+      <c r="G50" s="63"/>
+      <c r="H50" s="66" t="s">
+        <v>27</v>
+      </c>
+      <c r="I50" s="63"/>
+      <c r="J50" s="62" t="s">
+        <v>7</v>
+      </c>
+      <c r="K50" s="63"/>
+    </row>
+    <row r="51" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="65"/>
+      <c r="B51" s="31" t="str">
+        <f>RUBRICA!A6</f>
+        <v>3. Relaciona el Proyecto APT con sus intereses profesionales. *</v>
+      </c>
+      <c r="C51" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="D51" s="17" t="str">
+        <f t="shared" ref="D51:D53" si="17">IF($C51=CL,"X","")</f>
+        <v>X</v>
+      </c>
+      <c r="E51" s="17">
+        <f>IF(D51="X",100*0.05,"")</f>
+        <v>5</v>
+      </c>
+      <c r="F51" s="17" t="str">
+        <f t="shared" ref="F51:F53" si="18">IF($C51=L,"X","")</f>
+        <v/>
+      </c>
+      <c r="G51" s="17" t="str">
+        <f>IF(F51="X",60*0.05,"")</f>
+        <v/>
+      </c>
+      <c r="H51" s="17" t="str">
+        <f t="shared" ref="H51:H53" si="19">IF($C51=ML,"X","")</f>
+        <v/>
+      </c>
+      <c r="I51" s="17" t="str">
+        <f>IF(H51="X",30*0.05,"")</f>
+        <v/>
+      </c>
+      <c r="J51" s="17" t="str">
+        <f t="shared" ref="J51:J53" si="20">IF($C51=NL,"X","")</f>
+        <v/>
+      </c>
+      <c r="K51" s="17" t="str">
+        <f t="shared" ref="K51:K53" si="21">IF($J51="X",0,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="52" spans="1:11" ht="25.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="65"/>
+      <c r="B52" s="31" t="str">
+        <f>RUBRICA!A11</f>
+        <v>8. Expone el tema utilizando un lenguaje técnico disciplinar al presentar la propuesta y responde evidenciando un manejo de la información. *</v>
+      </c>
+      <c r="C52" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="D52" s="17" t="str">
+        <f t="shared" si="17"/>
+        <v>X</v>
+      </c>
+      <c r="E52" s="17">
+        <f>IF(D52="X",100*0.1,"")</f>
+        <v>10</v>
+      </c>
+      <c r="F52" s="17" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="G52" s="17" t="str">
+        <f>IF(F52="X",60*0.1,"")</f>
+        <v/>
+      </c>
+      <c r="H52" s="17" t="str">
+        <f t="shared" si="19"/>
+        <v/>
+      </c>
+      <c r="I52" s="17" t="str">
+        <f>IF(H52="X",30*0.1,"")</f>
+        <v/>
+      </c>
+      <c r="J52" s="17" t="str">
+        <f t="shared" si="20"/>
+        <v/>
+      </c>
+      <c r="K52" s="17" t="str">
+        <f t="shared" si="21"/>
+        <v/>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A53" s="65"/>
+      <c r="B53" s="31" t="str">
+        <f>RUBRICA!A13</f>
+        <v>10. Colaboración y trabajo en equipo *</v>
+      </c>
+      <c r="C53" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="D53" s="17" t="str">
+        <f t="shared" si="17"/>
+        <v>X</v>
+      </c>
+      <c r="E53" s="17">
+        <f>IF(D53="X",100*0.1,"")</f>
+        <v>10</v>
+      </c>
+      <c r="F53" s="17" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="G53" s="17" t="str">
+        <f>IF(F53="X",60*0.1,"")</f>
+        <v/>
+      </c>
+      <c r="H53" s="17" t="str">
+        <f t="shared" si="19"/>
+        <v/>
+      </c>
+      <c r="I53" s="17" t="str">
+        <f>IF(H53="X",30*0.1,"")</f>
+        <v/>
+      </c>
+      <c r="J53" s="17" t="str">
+        <f t="shared" si="20"/>
+        <v/>
+      </c>
+      <c r="K53" s="17" t="str">
+        <f t="shared" si="21"/>
+        <v/>
+      </c>
+    </row>
+    <row r="54" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="65"/>
+      <c r="B54" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="C54" s="19">
+        <f>E54+G54+I54+K54</f>
+        <v>25</v>
+      </c>
+      <c r="D54" s="20"/>
+      <c r="E54" s="20">
+        <f>SUM(E51:E53)</f>
+        <v>25</v>
+      </c>
+      <c r="F54" s="20"/>
+      <c r="G54" s="20">
+        <f>SUM(G51:G53)</f>
+        <v>0</v>
+      </c>
+      <c r="H54" s="20"/>
+      <c r="I54" s="20">
+        <f>SUM(I51:I53)</f>
+        <v>0</v>
+      </c>
+      <c r="J54" s="20"/>
+      <c r="K54" s="20">
+        <f>SUM(K52:K53)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="54"/>
+      <c r="B55" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C55" s="21">
+        <f>VLOOKUP(C54,ESCALA_TRAB_EQUIP!A1:B52,2,FALSE)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B56" s="23"/>
+      <c r="C56" s="24"/>
+    </row>
+    <row r="57" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B57" s="73" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B58" s="74" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B59" s="74" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B60" s="74" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B61" s="74" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B62" s="74" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B63" s="74" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B64" s="74" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B65" s="74" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B66" s="74" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="67" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B67" s="74" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="68" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="69" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="70" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B70" s="73" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="71" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="72" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="73" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="74" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="75" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="76" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="77" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="78" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="79" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="80" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="81" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="82" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="83" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2739,17 +3775,76 @@
     <row r="893" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="894" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="895" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="896" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="897" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="898" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="899" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="900" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="901" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="902" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="903" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="904" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="905" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="906" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="907" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="908" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="909" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="910" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="911" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="912" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="913" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="914" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="915" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="916" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="917" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="918" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="919" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="920" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="921" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="922" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="923" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="924" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="925" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="926" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="A11:A22"/>
+  <mergeCells count="35">
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="C36:K37"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="D38:K38"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="J39:K39"/>
+    <mergeCell ref="A36:A44"/>
+    <mergeCell ref="A24:A32"/>
+    <mergeCell ref="E2:E3"/>
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="D11:K11"/>
     <mergeCell ref="F12:G12"/>
     <mergeCell ref="H12:I12"/>
     <mergeCell ref="J12:K12"/>
+    <mergeCell ref="A11:A21"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:K25"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="D26:K26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="D49:K49"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="F50:G50"/>
+    <mergeCell ref="H50:I50"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="C47:K48"/>
+    <mergeCell ref="J50:K50"/>
+    <mergeCell ref="A47:A55"/>
   </mergeCells>
-  <conditionalFormatting sqref="C4:C6">
+  <conditionalFormatting sqref="C4:E6">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
       <formula>4</formula>
     </cfRule>
@@ -2758,14 +3853,13 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Error de Ingreso - Nota debe estar entre 1,0 y 7,0" sqref="C4:C6" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Error de Ingreso - Nota debe estar entre 1,0 y 7,0" sqref="C4:E6" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>1</formula1>
       <formula2>7</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
-  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
@@ -2773,238 +3867,11 @@
           <x14:formula1>
             <xm:f>'RELEVANCIA-PUNTAJE'!$B$2:$E$2</xm:f>
           </x14:formula1>
-          <xm:sqref>C13:C20</xm:sqref>
+          <xm:sqref>C40:C42 C13:C19 C28:C30 C51:C53</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B396D1B-8A63-4A90-BA20-D34AC13A3962}">
-  <dimension ref="A1:F11"/>
-  <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="113" zoomScaleNormal="113" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="6" width="38.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="50" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="52" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="50" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="51"/>
-      <c r="B2" s="56" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="56" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="51"/>
-    </row>
-    <row r="3" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="51"/>
-      <c r="B3" s="57"/>
-      <c r="C3" s="57"/>
-      <c r="D3" s="36">
-        <v>-0.3</v>
-      </c>
-      <c r="E3" s="36">
-        <v>0</v>
-      </c>
-      <c r="F3" s="55"/>
-    </row>
-    <row r="4" spans="1:6" ht="46" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="F4" s="23">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="61" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="C5" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="D5" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="E5" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="F5" s="23">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="91" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="B6" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="C6" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="D6" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="E6" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="F6" s="23">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="46" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="B7" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="C7" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="D7" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="E7" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="F7" s="23">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.2">
-      <c r="A8" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="F8" s="37">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="61" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="B9" s="24" t="s">
-        <v>54</v>
-      </c>
-      <c r="C9" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="D9" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="E9" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="F9" s="23">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="61" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="38" t="s">
-        <v>58</v>
-      </c>
-      <c r="B10" s="38" t="s">
-        <v>59</v>
-      </c>
-      <c r="C10" s="38" t="s">
-        <v>60</v>
-      </c>
-      <c r="D10" s="38" t="s">
-        <v>61</v>
-      </c>
-      <c r="E10" s="38" t="s">
-        <v>62</v>
-      </c>
-      <c r="F10" s="31">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="81.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="B11" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="E11" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="F11" s="35">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:F3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -3013,7 +3880,7 @@
   <dimension ref="A1:B1000"/>
   <sheetViews>
     <sheetView topLeftCell="A146" workbookViewId="0">
-      <selection sqref="A1:B202"/>
+      <selection activeCell="A153" sqref="A153:B162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3074,7 +3941,7 @@
         <v>2.5</v>
       </c>
       <c r="B7">
-        <v>1.1000000000000001</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -3098,7 +3965,7 @@
         <v>4</v>
       </c>
       <c r="B10">
-        <v>1.2</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -3106,7 +3973,7 @@
         <v>4.5</v>
       </c>
       <c r="B11">
-        <v>1.2</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -3122,7 +3989,7 @@
         <v>5.5</v>
       </c>
       <c r="B13">
-        <v>1.3</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -3130,7 +3997,7 @@
         <v>6</v>
       </c>
       <c r="B14">
-        <v>1.3</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -3138,7 +4005,7 @@
         <v>6.5</v>
       </c>
       <c r="B15">
-        <v>1.3</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -3146,7 +4013,7 @@
         <v>7</v>
       </c>
       <c r="B16">
-        <v>1.4</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -3154,7 +4021,7 @@
         <v>7.5</v>
       </c>
       <c r="B17">
-        <v>1.4</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -3162,7 +4029,7 @@
         <v>8</v>
       </c>
       <c r="B18">
-        <v>1.4</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -3170,7 +4037,7 @@
         <v>8.5</v>
       </c>
       <c r="B19">
-        <v>1.4</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -3178,7 +4045,7 @@
         <v>9</v>
       </c>
       <c r="B20">
-        <v>1.5</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3186,7 +4053,7 @@
         <v>9.5</v>
       </c>
       <c r="B21">
-        <v>1.5</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3194,7 +4061,7 @@
         <v>10</v>
       </c>
       <c r="B22">
-        <v>1.5</v>
+        <v>1.7</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3202,7 +4069,7 @@
         <v>10.5</v>
       </c>
       <c r="B23">
-        <v>1.5</v>
+        <v>1.7</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3210,7 +4077,7 @@
         <v>11</v>
       </c>
       <c r="B24">
-        <v>1.6</v>
+        <v>1.7</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3218,7 +4085,7 @@
         <v>11.5</v>
       </c>
       <c r="B25">
-        <v>1.6</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3226,7 +4093,7 @@
         <v>12</v>
       </c>
       <c r="B26">
-        <v>1.6</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3234,7 +4101,7 @@
         <v>12.5</v>
       </c>
       <c r="B27">
-        <v>1.6</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3242,7 +4109,7 @@
         <v>13</v>
       </c>
       <c r="B28">
-        <v>1.7</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3250,7 +4117,7 @@
         <v>13.5</v>
       </c>
       <c r="B29">
-        <v>1.7</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3258,7 +4125,7 @@
         <v>14</v>
       </c>
       <c r="B30">
-        <v>1.7</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3266,7 +4133,7 @@
         <v>14.5</v>
       </c>
       <c r="B31">
-        <v>1.7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3274,7 +4141,7 @@
         <v>15</v>
       </c>
       <c r="B32">
-        <v>1.8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3282,7 +4149,7 @@
         <v>15.5</v>
       </c>
       <c r="B33">
-        <v>1.8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3290,7 +4157,7 @@
         <v>16</v>
       </c>
       <c r="B34">
-        <v>1.8</v>
+        <v>2.1</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3298,7 +4165,7 @@
         <v>16.5</v>
       </c>
       <c r="B35">
-        <v>1.8</v>
+        <v>2.1</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3306,7 +4173,7 @@
         <v>17</v>
       </c>
       <c r="B36">
-        <v>1.9</v>
+        <v>2.1</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3314,7 +4181,7 @@
         <v>17.5</v>
       </c>
       <c r="B37">
-        <v>1.9</v>
+        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3322,7 +4189,7 @@
         <v>18</v>
       </c>
       <c r="B38">
-        <v>1.9</v>
+        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3330,7 +4197,7 @@
         <v>18.5</v>
       </c>
       <c r="B39">
-        <v>1.9</v>
+        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3338,7 +4205,7 @@
         <v>19</v>
       </c>
       <c r="B40">
-        <v>2</v>
+        <v>2.2999999999999998</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3346,7 +4213,7 @@
         <v>19.5</v>
       </c>
       <c r="B41">
-        <v>2</v>
+        <v>2.2999999999999998</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3354,7 +4221,7 @@
         <v>20</v>
       </c>
       <c r="B42">
-        <v>2</v>
+        <v>2.2999999999999998</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3362,7 +4229,7 @@
         <v>20.5</v>
       </c>
       <c r="B43">
-        <v>2</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3370,7 +4237,7 @@
         <v>21</v>
       </c>
       <c r="B44">
-        <v>2.1</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3378,7 +4245,7 @@
         <v>21.5</v>
       </c>
       <c r="B45">
-        <v>2.1</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3386,7 +4253,7 @@
         <v>22</v>
       </c>
       <c r="B46">
-        <v>2.1</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3394,7 +4261,7 @@
         <v>22.5</v>
       </c>
       <c r="B47">
-        <v>2.1</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3402,7 +4269,7 @@
         <v>23</v>
       </c>
       <c r="B48">
-        <v>2.2000000000000002</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3410,7 +4277,7 @@
         <v>23.5</v>
       </c>
       <c r="B49">
-        <v>2.2000000000000002</v>
+        <v>2.6</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3418,7 +4285,7 @@
         <v>24</v>
       </c>
       <c r="B50">
-        <v>2.2000000000000002</v>
+        <v>2.6</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3426,7 +4293,7 @@
         <v>24.5</v>
       </c>
       <c r="B51">
-        <v>2.2000000000000002</v>
+        <v>2.6</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3434,7 +4301,7 @@
         <v>25</v>
       </c>
       <c r="B52">
-        <v>2.2999999999999998</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3442,7 +4309,7 @@
         <v>25.5</v>
       </c>
       <c r="B53">
-        <v>2.2999999999999998</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3450,7 +4317,7 @@
         <v>26</v>
       </c>
       <c r="B54">
-        <v>2.2999999999999998</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3458,7 +4325,7 @@
         <v>26.5</v>
       </c>
       <c r="B55">
-        <v>2.2999999999999998</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3466,7 +4333,7 @@
         <v>27</v>
       </c>
       <c r="B56">
-        <v>2.4</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3474,7 +4341,7 @@
         <v>27.5</v>
       </c>
       <c r="B57">
-        <v>2.4</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3482,7 +4349,7 @@
         <v>28</v>
       </c>
       <c r="B58">
-        <v>2.4</v>
+        <v>2.9</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3490,7 +4357,7 @@
         <v>28.5</v>
       </c>
       <c r="B59">
-        <v>2.4</v>
+        <v>2.9</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3498,7 +4365,7 @@
         <v>29</v>
       </c>
       <c r="B60">
-        <v>2.5</v>
+        <v>2.9</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3506,7 +4373,7 @@
         <v>29.5</v>
       </c>
       <c r="B61">
-        <v>2.5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3514,7 +4381,7 @@
         <v>30</v>
       </c>
       <c r="B62">
-        <v>2.5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3522,7 +4389,7 @@
         <v>30.5</v>
       </c>
       <c r="B63">
-        <v>2.5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3530,7 +4397,7 @@
         <v>31</v>
       </c>
       <c r="B64">
-        <v>2.6</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3538,7 +4405,7 @@
         <v>31.5</v>
       </c>
       <c r="B65">
-        <v>2.6</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3546,7 +4413,7 @@
         <v>32</v>
       </c>
       <c r="B66">
-        <v>2.6</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3554,7 +4421,7 @@
         <v>32.5</v>
       </c>
       <c r="B67">
-        <v>2.6</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3562,7 +4429,7 @@
         <v>33</v>
       </c>
       <c r="B68">
-        <v>2.7</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3570,7 +4437,7 @@
         <v>33.5</v>
       </c>
       <c r="B69">
-        <v>2.7</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3578,7 +4445,7 @@
         <v>34</v>
       </c>
       <c r="B70">
-        <v>2.7</v>
+        <v>3.3</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3586,7 +4453,7 @@
         <v>34.5</v>
       </c>
       <c r="B71">
-        <v>2.7</v>
+        <v>3.3</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3594,7 +4461,7 @@
         <v>35</v>
       </c>
       <c r="B72">
-        <v>2.8</v>
+        <v>3.3</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3602,7 +4469,7 @@
         <v>35.5</v>
       </c>
       <c r="B73">
-        <v>2.8</v>
+        <v>3.4</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3610,7 +4477,7 @@
         <v>36</v>
       </c>
       <c r="B74">
-        <v>2.8</v>
+        <v>3.4</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3618,7 +4485,7 @@
         <v>36.5</v>
       </c>
       <c r="B75">
-        <v>2.8</v>
+        <v>3.4</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3626,7 +4493,7 @@
         <v>37</v>
       </c>
       <c r="B76">
-        <v>2.9</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3634,7 +4501,7 @@
         <v>37.5</v>
       </c>
       <c r="B77">
-        <v>2.9</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3642,7 +4509,7 @@
         <v>38</v>
       </c>
       <c r="B78">
-        <v>2.9</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3650,7 +4517,7 @@
         <v>38.5</v>
       </c>
       <c r="B79">
-        <v>2.9</v>
+        <v>3.6</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3658,7 +4525,7 @@
         <v>39</v>
       </c>
       <c r="B80">
-        <v>3</v>
+        <v>3.6</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3666,7 +4533,7 @@
         <v>39.5</v>
       </c>
       <c r="B81">
-        <v>3</v>
+        <v>3.6</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3674,7 +4541,7 @@
         <v>40</v>
       </c>
       <c r="B82">
-        <v>3</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3682,7 +4549,7 @@
         <v>40.5</v>
       </c>
       <c r="B83">
-        <v>3</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3690,7 +4557,7 @@
         <v>41</v>
       </c>
       <c r="B84">
-        <v>3.1</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3698,7 +4565,7 @@
         <v>41.5</v>
       </c>
       <c r="B85">
-        <v>3.1</v>
+        <v>3.8</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3706,7 +4573,7 @@
         <v>42</v>
       </c>
       <c r="B86">
-        <v>3.1</v>
+        <v>3.8</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3714,7 +4581,7 @@
         <v>42.5</v>
       </c>
       <c r="B87">
-        <v>3.1</v>
+        <v>3.8</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3722,7 +4589,7 @@
         <v>43</v>
       </c>
       <c r="B88">
-        <v>3.2</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3730,7 +4597,7 @@
         <v>43.5</v>
       </c>
       <c r="B89">
-        <v>3.2</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3738,7 +4605,7 @@
         <v>44</v>
       </c>
       <c r="B90">
-        <v>3.2</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3746,7 +4613,7 @@
         <v>44.5</v>
       </c>
       <c r="B91">
-        <v>3.2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3754,7 +4621,7 @@
         <v>45</v>
       </c>
       <c r="B92">
-        <v>3.3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3762,7 +4629,7 @@
         <v>45.5</v>
       </c>
       <c r="B93">
-        <v>3.3</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3770,7 +4637,7 @@
         <v>46</v>
       </c>
       <c r="B94">
-        <v>3.3</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3778,7 +4645,7 @@
         <v>46.5</v>
       </c>
       <c r="B95">
-        <v>3.3</v>
+        <v>4.2</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3786,7 +4653,7 @@
         <v>47</v>
       </c>
       <c r="B96">
-        <v>3.4</v>
+        <v>4.2</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3794,7 +4661,7 @@
         <v>47.5</v>
       </c>
       <c r="B97">
-        <v>3.4</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3802,7 +4669,7 @@
         <v>48</v>
       </c>
       <c r="B98">
-        <v>3.4</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3810,7 +4677,7 @@
         <v>48.5</v>
       </c>
       <c r="B99">
-        <v>3.4</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3818,7 +4685,7 @@
         <v>49</v>
       </c>
       <c r="B100">
-        <v>3.5</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3826,7 +4693,7 @@
         <v>49.5</v>
       </c>
       <c r="B101">
-        <v>3.5</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3834,7 +4701,7 @@
         <v>50</v>
       </c>
       <c r="B102">
-        <v>3.5</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3842,7 +4709,7 @@
         <v>50.5</v>
       </c>
       <c r="B103">
-        <v>3.5</v>
+        <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3850,7 +4717,7 @@
         <v>51</v>
       </c>
       <c r="B104">
-        <v>3.6</v>
+        <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3858,7 +4725,7 @@
         <v>51.5</v>
       </c>
       <c r="B105">
-        <v>3.6</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3866,7 +4733,7 @@
         <v>52</v>
       </c>
       <c r="B106">
-        <v>3.6</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3874,7 +4741,7 @@
         <v>52.5</v>
       </c>
       <c r="B107">
-        <v>3.6</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3882,7 +4749,7 @@
         <v>53</v>
       </c>
       <c r="B108">
-        <v>3.7</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3890,7 +4757,7 @@
         <v>53.5</v>
       </c>
       <c r="B109">
-        <v>3.7</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3898,7 +4765,7 @@
         <v>54</v>
       </c>
       <c r="B110">
-        <v>3.7</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3906,7 +4773,7 @@
         <v>54.5</v>
       </c>
       <c r="B111">
-        <v>3.7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3914,7 +4781,7 @@
         <v>55</v>
       </c>
       <c r="B112">
-        <v>3.8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3922,7 +4789,7 @@
         <v>55.5</v>
       </c>
       <c r="B113">
-        <v>3.8</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3930,7 +4797,7 @@
         <v>56</v>
       </c>
       <c r="B114">
-        <v>3.8</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3938,7 +4805,7 @@
         <v>56.5</v>
       </c>
       <c r="B115">
-        <v>3.8</v>
+        <v>5.2</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3946,7 +4813,7 @@
         <v>57</v>
       </c>
       <c r="B116">
-        <v>3.9</v>
+        <v>5.2</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3954,7 +4821,7 @@
         <v>57.5</v>
       </c>
       <c r="B117">
-        <v>3.9</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3962,7 +4829,7 @@
         <v>58</v>
       </c>
       <c r="B118">
-        <v>3.9</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3970,7 +4837,7 @@
         <v>58.5</v>
       </c>
       <c r="B119">
-        <v>3.9</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="120" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3978,7 +4845,7 @@
         <v>59</v>
       </c>
       <c r="B120">
-        <v>4</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="121" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3986,7 +4853,7 @@
         <v>59.5</v>
       </c>
       <c r="B121">
-        <v>4</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="122" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3994,7 +4861,7 @@
         <v>60</v>
       </c>
       <c r="B122">
-        <v>4</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="123" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4002,7 +4869,7 @@
         <v>60.5</v>
       </c>
       <c r="B123">
-        <v>4</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="124" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4010,7 +4877,7 @@
         <v>61</v>
       </c>
       <c r="B124">
-        <v>4.0999999999999996</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="125" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4018,7 +4885,7 @@
         <v>61.5</v>
       </c>
       <c r="B125">
-        <v>4.0999999999999996</v>
+        <v>5.7</v>
       </c>
     </row>
     <row r="126" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4026,7 +4893,7 @@
         <v>62</v>
       </c>
       <c r="B126">
-        <v>4.2</v>
+        <v>5.7</v>
       </c>
     </row>
     <row r="127" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4034,7 +4901,7 @@
         <v>62.5</v>
       </c>
       <c r="B127">
-        <v>4.2</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="128" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4042,7 +4909,7 @@
         <v>63</v>
       </c>
       <c r="B128">
-        <v>4.2</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4050,7 +4917,7 @@
         <v>63.5</v>
       </c>
       <c r="B129">
-        <v>4.3</v>
+        <v>5.9</v>
       </c>
     </row>
     <row r="130" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4058,7 +4925,7 @@
         <v>64</v>
       </c>
       <c r="B130">
-        <v>4.3</v>
+        <v>5.9</v>
       </c>
     </row>
     <row r="131" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4066,7 +4933,7 @@
         <v>64.5</v>
       </c>
       <c r="B131">
-        <v>4.3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="132" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4074,7 +4941,7 @@
         <v>65</v>
       </c>
       <c r="B132">
-        <v>4.4000000000000004</v>
+        <v>6</v>
       </c>
     </row>
     <row r="133" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4082,7 +4949,7 @@
         <v>65.5</v>
       </c>
       <c r="B133">
-        <v>4.4000000000000004</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="134" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4090,7 +4957,7 @@
         <v>66</v>
       </c>
       <c r="B134">
-        <v>4.5</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="135" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4098,7 +4965,7 @@
         <v>66.5</v>
       </c>
       <c r="B135">
-        <v>4.5</v>
+        <v>6.2</v>
       </c>
     </row>
     <row r="136" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4106,7 +4973,7 @@
         <v>67</v>
       </c>
       <c r="B136">
-        <v>4.5</v>
+        <v>6.2</v>
       </c>
     </row>
     <row r="137" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4114,7 +4981,7 @@
         <v>67.5</v>
       </c>
       <c r="B137">
-        <v>4.5999999999999996</v>
+        <v>6.3</v>
       </c>
     </row>
     <row r="138" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4122,7 +4989,7 @@
         <v>68</v>
       </c>
       <c r="B138">
-        <v>4.5999999999999996</v>
+        <v>6.3</v>
       </c>
     </row>
     <row r="139" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4130,7 +4997,7 @@
         <v>68.5</v>
       </c>
       <c r="B139">
-        <v>4.5999999999999996</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="140" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4138,7 +5005,7 @@
         <v>69</v>
       </c>
       <c r="B140">
-        <v>4.7</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="141" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4146,7 +5013,7 @@
         <v>69.5</v>
       </c>
       <c r="B141">
-        <v>4.7</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="142" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4154,7 +5021,7 @@
         <v>70</v>
       </c>
       <c r="B142">
-        <v>4.8</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="143" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4162,7 +5029,7 @@
         <v>70.5</v>
       </c>
       <c r="B143">
-        <v>4.8</v>
+        <v>6.6</v>
       </c>
     </row>
     <row r="144" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4170,7 +5037,7 @@
         <v>71</v>
       </c>
       <c r="B144">
-        <v>4.8</v>
+        <v>6.6</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4178,7 +5045,7 @@
         <v>71.5</v>
       </c>
       <c r="B145">
-        <v>4.9000000000000004</v>
+        <v>6.7</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4186,7 +5053,7 @@
         <v>72</v>
       </c>
       <c r="B146">
-        <v>4.9000000000000004</v>
+        <v>6.7</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4194,7 +5061,7 @@
         <v>72.5</v>
       </c>
       <c r="B147">
-        <v>4.9000000000000004</v>
+        <v>6.8</v>
       </c>
     </row>
     <row r="148" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4202,7 +5069,7 @@
         <v>73</v>
       </c>
       <c r="B148">
-        <v>5</v>
+        <v>6.8</v>
       </c>
     </row>
     <row r="149" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4210,7 +5077,7 @@
         <v>73.5</v>
       </c>
       <c r="B149">
-        <v>5</v>
+        <v>6.9</v>
       </c>
     </row>
     <row r="150" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4218,7 +5085,7 @@
         <v>74</v>
       </c>
       <c r="B150">
-        <v>5.0999999999999996</v>
+        <v>6.9</v>
       </c>
     </row>
     <row r="151" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4226,7 +5093,7 @@
         <v>74.5</v>
       </c>
       <c r="B151">
-        <v>5.0999999999999996</v>
+        <v>7</v>
       </c>
     </row>
     <row r="152" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4234,415 +5101,65 @@
         <v>75</v>
       </c>
       <c r="B152">
-        <v>5.0999999999999996</v>
-      </c>
-    </row>
-    <row r="153" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A153">
-        <v>75.5</v>
-      </c>
-      <c r="B153">
-        <v>5.2</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A154">
-        <v>76</v>
-      </c>
-      <c r="B154">
-        <v>5.2</v>
-      </c>
-    </row>
-    <row r="155" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A155">
-        <v>76.5</v>
-      </c>
-      <c r="B155">
-        <v>5.2</v>
-      </c>
-    </row>
-    <row r="156" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A156">
-        <v>77</v>
-      </c>
-      <c r="B156">
-        <v>5.3</v>
-      </c>
-    </row>
-    <row r="157" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A157">
-        <v>77.5</v>
-      </c>
-      <c r="B157">
-        <v>5.3</v>
-      </c>
-    </row>
-    <row r="158" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A158">
-        <v>78</v>
-      </c>
-      <c r="B158">
-        <v>5.4</v>
-      </c>
-    </row>
-    <row r="159" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A159">
-        <v>78.5</v>
-      </c>
-      <c r="B159">
-        <v>5.4</v>
-      </c>
-    </row>
-    <row r="160" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A160">
-        <v>79</v>
-      </c>
-      <c r="B160">
-        <v>5.4</v>
-      </c>
-    </row>
-    <row r="161" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A161">
-        <v>79.5</v>
-      </c>
-      <c r="B161">
-        <v>5.5</v>
-      </c>
-    </row>
-    <row r="162" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A162">
-        <v>80</v>
-      </c>
-      <c r="B162">
-        <v>5.5</v>
-      </c>
-    </row>
-    <row r="163" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A163">
-        <v>80.5</v>
-      </c>
-      <c r="B163">
-        <v>5.5</v>
-      </c>
-    </row>
-    <row r="164" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A164">
-        <v>81</v>
-      </c>
-      <c r="B164">
-        <v>5.6</v>
-      </c>
-    </row>
-    <row r="165" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A165">
-        <v>81.5</v>
-      </c>
-      <c r="B165">
-        <v>5.6</v>
-      </c>
-    </row>
-    <row r="166" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A166">
-        <v>82</v>
-      </c>
-      <c r="B166">
-        <v>5.7</v>
-      </c>
-    </row>
-    <row r="167" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A167">
-        <v>82.5</v>
-      </c>
-      <c r="B167">
-        <v>5.7</v>
-      </c>
-    </row>
-    <row r="168" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A168">
-        <v>83</v>
-      </c>
-      <c r="B168">
-        <v>5.7</v>
-      </c>
-    </row>
-    <row r="169" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A169">
-        <v>83.5</v>
-      </c>
-      <c r="B169">
-        <v>5.8</v>
-      </c>
-    </row>
-    <row r="170" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A170">
-        <v>84</v>
-      </c>
-      <c r="B170">
-        <v>5.8</v>
-      </c>
-    </row>
-    <row r="171" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A171">
-        <v>84.5</v>
-      </c>
-      <c r="B171">
-        <v>5.8</v>
-      </c>
-    </row>
-    <row r="172" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A172">
-        <v>85</v>
-      </c>
-      <c r="B172">
-        <v>5.9</v>
-      </c>
-    </row>
-    <row r="173" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A173">
-        <v>85.5</v>
-      </c>
-      <c r="B173">
-        <v>5.9</v>
-      </c>
-    </row>
-    <row r="174" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A174">
-        <v>86</v>
-      </c>
-      <c r="B174">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="175" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A175">
-        <v>86.5</v>
-      </c>
-      <c r="B175">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="176" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A176">
-        <v>87</v>
-      </c>
-      <c r="B176">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="177" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A177">
-        <v>87.5</v>
-      </c>
-      <c r="B177">
-        <v>6.1</v>
-      </c>
-    </row>
-    <row r="178" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A178">
-        <v>88</v>
-      </c>
-      <c r="B178">
-        <v>6.1</v>
-      </c>
-    </row>
-    <row r="179" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A179">
-        <v>88.5</v>
-      </c>
-      <c r="B179">
-        <v>6.1</v>
-      </c>
-    </row>
-    <row r="180" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A180">
-        <v>89</v>
-      </c>
-      <c r="B180">
-        <v>6.2</v>
-      </c>
-    </row>
-    <row r="181" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A181">
-        <v>89.5</v>
-      </c>
-      <c r="B181">
-        <v>6.2</v>
-      </c>
-    </row>
-    <row r="182" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A182">
-        <v>90</v>
-      </c>
-      <c r="B182">
-        <v>6.3</v>
-      </c>
-    </row>
-    <row r="183" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A183">
-        <v>90.5</v>
-      </c>
-      <c r="B183">
-        <v>6.3</v>
-      </c>
-    </row>
-    <row r="184" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A184">
-        <v>91</v>
-      </c>
-      <c r="B184">
-        <v>6.3</v>
-      </c>
-    </row>
-    <row r="185" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A185">
-        <v>91.5</v>
-      </c>
-      <c r="B185">
-        <v>6.4</v>
-      </c>
-    </row>
-    <row r="186" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A186">
-        <v>92</v>
-      </c>
-      <c r="B186">
-        <v>6.4</v>
-      </c>
-    </row>
-    <row r="187" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A187">
-        <v>92.5</v>
-      </c>
-      <c r="B187">
-        <v>6.4</v>
-      </c>
-    </row>
-    <row r="188" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A188">
-        <v>93</v>
-      </c>
-      <c r="B188">
-        <v>6.5</v>
-      </c>
-    </row>
-    <row r="189" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A189">
-        <v>93.5</v>
-      </c>
-      <c r="B189">
-        <v>6.5</v>
-      </c>
-    </row>
-    <row r="190" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A190">
-        <v>94</v>
-      </c>
-      <c r="B190">
-        <v>6.6</v>
-      </c>
-    </row>
-    <row r="191" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A191">
-        <v>94.5</v>
-      </c>
-      <c r="B191">
-        <v>6.6</v>
-      </c>
-    </row>
-    <row r="192" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A192">
-        <v>95</v>
-      </c>
-      <c r="B192">
-        <v>6.6</v>
-      </c>
-    </row>
-    <row r="193" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A193">
-        <v>95.5</v>
-      </c>
-      <c r="B193">
-        <v>6.7</v>
-      </c>
-    </row>
-    <row r="194" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A194">
-        <v>96</v>
-      </c>
-      <c r="B194">
-        <v>6.7</v>
-      </c>
-    </row>
-    <row r="195" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A195">
-        <v>96.5</v>
-      </c>
-      <c r="B195">
-        <v>6.7</v>
-      </c>
-    </row>
-    <row r="196" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A196">
-        <v>97</v>
-      </c>
-      <c r="B196">
-        <v>6.8</v>
-      </c>
-    </row>
-    <row r="197" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A197">
-        <v>97.5</v>
-      </c>
-      <c r="B197">
-        <v>6.8</v>
-      </c>
-    </row>
-    <row r="198" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A198">
-        <v>98</v>
-      </c>
-      <c r="B198">
-        <v>6.9</v>
-      </c>
-    </row>
-    <row r="199" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A199">
-        <v>98.5</v>
-      </c>
-      <c r="B199">
-        <v>6.9</v>
-      </c>
-    </row>
-    <row r="200" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A200">
-        <v>99</v>
-      </c>
-      <c r="B200">
-        <v>6.9</v>
-      </c>
-    </row>
-    <row r="201" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A201">
-        <v>99.5</v>
-      </c>
-      <c r="B201">
         <v>7</v>
       </c>
     </row>
-    <row r="202" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A202">
-        <v>100</v>
-      </c>
-      <c r="B202">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="203" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="204" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="205" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="206" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="207" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="208" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="153" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="154" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="155" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="156" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="157" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="158" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="159" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="160" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="161" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="162" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="163" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="164" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="165" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="166" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="167" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="168" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="169" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="170" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="171" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="172" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="173" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="174" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="175" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="176" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="177" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="178" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="179" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="180" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="181" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="182" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="183" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="184" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="185" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="186" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="187" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="188" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="189" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="190" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="192" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="193" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="194" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="195" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="196" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="197" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="198" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="199" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="200" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="201" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="202" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="203" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="204" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="205" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="206" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="207" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="208" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="209" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="210" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="211" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6840,8 +7357,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection sqref="A1:B52"/>
+    <sheetView topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="A153" sqref="A153:B162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -8237,61 +8754,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="9"/>
     </row>
     <row r="2" spans="1:5" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="59"/>
-      <c r="B2" s="9" t="s">
+      <c r="A2" s="72"/>
+      <c r="B2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="28" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" s="11" t="s">
+      <c r="D2" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="12" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="33" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="13">
+      <c r="B3" s="14">
         <v>4</v>
       </c>
-      <c r="C3" s="13">
+      <c r="C3" s="14">
         <v>3</v>
       </c>
-      <c r="D3" s="13">
+      <c r="D3" s="14">
         <v>2</v>
       </c>
-      <c r="E3" s="13">
+      <c r="E3" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
+      <c r="A4" s="13"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
     </row>
     <row r="5" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="12"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
+      <c r="A5" s="13"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>